<commit_message>
fixed base spelling for ogbi1239-1
</commit_message>
<xml_diff>
--- a/raw/xlsx/numerals-ogbi1239-1.xlsx
+++ b/raw/xlsx/numerals-ogbi1239-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Documents/Developments/shh_git/numeralbank/numerals/raw/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6E1142-5F66-6146-96EF-DCEC62A5DAB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E0FA84-E682-B940-94AD-D883EF7E0ECD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="760" windowWidth="22460" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="760" windowWidth="22460" windowHeight="14260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>Ogbia.htm</t>
   </si>
   <si>
-    <t>Vigesimal</t>
-  </si>
-  <si>
     <t>Merosobo</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>(30 - 1)</t>
+  </si>
+  <si>
+    <t>vigesimal</t>
   </si>
 </sst>
 </file>
@@ -741,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -778,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="3"/>
@@ -789,7 +789,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="3"/>
@@ -800,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="3"/>
@@ -811,7 +811,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="3"/>
@@ -822,7 +822,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="3"/>
@@ -833,7 +833,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="3"/>
@@ -844,7 +844,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="3"/>
@@ -855,7 +855,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="3"/>
@@ -866,10 +866,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>38</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -879,7 +879,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -890,10 +890,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -903,7 +903,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -914,10 +914,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -927,7 +927,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -938,7 +938,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="3"/>
@@ -949,7 +949,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="7"/>
@@ -960,7 +960,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="3"/>
@@ -970,7 +970,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="7"/>
@@ -980,7 +980,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="17"/>
     </row>
@@ -989,10 +989,10 @@
         <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1000,10 +1000,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>51</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1011,10 +1011,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1022,10 +1022,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1033,7 +1033,7 @@
         <v>20</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1043,7 +1043,7 @@
         <v>21</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="18"/>
     </row>
@@ -1052,7 +1052,7 @@
         <v>22</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="18"/>
     </row>
@@ -1061,7 +1061,7 @@
         <v>23</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="18"/>
     </row>
@@ -1070,7 +1070,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="18"/>
     </row>
@@ -1079,7 +1079,7 @@
         <v>25</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="18"/>
     </row>
@@ -1088,7 +1088,7 @@
         <v>26</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="18"/>
     </row>
@@ -1097,7 +1097,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>20</v>
@@ -1108,7 +1108,7 @@
         <v>28</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="7"/>
     </row>
@@ -1117,10 +1117,10 @@
         <v>28</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1128,7 +1128,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="7"/>
     </row>
@@ -1137,10 +1137,10 @@
         <v>29</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1148,7 +1148,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="14"/>
     </row>
@@ -1157,10 +1157,10 @@
         <v>40</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>20</v>
@@ -1171,7 +1171,7 @@
         <v>50</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1181,7 +1181,7 @@
         <v>50</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -1191,10 +1191,10 @@
         <v>60</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="D41" s="7"/>
     </row>
@@ -1203,7 +1203,7 @@
         <v>70</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C42" s="7"/>
     </row>
@@ -1212,10 +1212,10 @@
         <v>80</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="D43" s="7"/>
     </row>
@@ -1224,7 +1224,7 @@
         <v>90</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" s="7"/>
     </row>
@@ -1233,10 +1233,10 @@
         <v>100</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="17" t="s">
         <v>79</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1244,7 +1244,7 @@
         <v>200</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="7"/>
     </row>
@@ -1253,7 +1253,7 @@
         <v>400</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -1263,7 +1263,7 @@
         <v>800</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="7"/>
     </row>
@@ -1272,7 +1272,7 @@
         <v>1000</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49" s="7"/>
     </row>
@@ -1281,7 +1281,7 @@
         <v>2000</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" s="7"/>
     </row>
@@ -1317,7 +1317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1348,7 +1348,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1372,7 +1372,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1380,7 +1380,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1388,7 +1388,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1396,7 +1396,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
@@ -1416,7 +1416,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1432,7 +1432,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1440,7 +1440,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to Glottolog v4.5 (#191)
* updated to Glottolog v4.5

* fixed base spelling for ogbi1239-1
</commit_message>
<xml_diff>
--- a/raw/xlsx/numerals-ogbi1239-1.xlsx
+++ b/raw/xlsx/numerals-ogbi1239-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Documents/Developments/shh_git/numeralbank/numerals/raw/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6E1142-5F66-6146-96EF-DCEC62A5DAB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E0FA84-E682-B940-94AD-D883EF7E0ECD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="760" windowWidth="22460" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="760" windowWidth="22460" windowHeight="14260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>Ogbia.htm</t>
   </si>
   <si>
-    <t>Vigesimal</t>
-  </si>
-  <si>
     <t>Merosobo</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>(30 - 1)</t>
+  </si>
+  <si>
+    <t>vigesimal</t>
   </si>
 </sst>
 </file>
@@ -741,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -778,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="3"/>
@@ -789,7 +789,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="3"/>
@@ -800,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="3"/>
@@ -811,7 +811,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="3"/>
@@ -822,7 +822,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="3"/>
@@ -833,7 +833,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="3"/>
@@ -844,7 +844,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="3"/>
@@ -855,7 +855,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="3"/>
@@ -866,10 +866,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>38</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -879,7 +879,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -890,10 +890,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -903,7 +903,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -914,10 +914,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -927,7 +927,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -938,7 +938,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="3"/>
@@ -949,7 +949,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="7"/>
@@ -960,7 +960,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="3"/>
@@ -970,7 +970,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="7"/>
@@ -980,7 +980,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="17"/>
     </row>
@@ -989,10 +989,10 @@
         <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1000,10 +1000,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>51</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1011,10 +1011,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1022,10 +1022,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1033,7 +1033,7 @@
         <v>20</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1043,7 +1043,7 @@
         <v>21</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="18"/>
     </row>
@@ -1052,7 +1052,7 @@
         <v>22</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="18"/>
     </row>
@@ -1061,7 +1061,7 @@
         <v>23</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="18"/>
     </row>
@@ -1070,7 +1070,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="18"/>
     </row>
@@ -1079,7 +1079,7 @@
         <v>25</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="18"/>
     </row>
@@ -1088,7 +1088,7 @@
         <v>26</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="18"/>
     </row>
@@ -1097,7 +1097,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>20</v>
@@ -1108,7 +1108,7 @@
         <v>28</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="7"/>
     </row>
@@ -1117,10 +1117,10 @@
         <v>28</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1128,7 +1128,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="7"/>
     </row>
@@ -1137,10 +1137,10 @@
         <v>29</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1148,7 +1148,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="14"/>
     </row>
@@ -1157,10 +1157,10 @@
         <v>40</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>20</v>
@@ -1171,7 +1171,7 @@
         <v>50</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1181,7 +1181,7 @@
         <v>50</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -1191,10 +1191,10 @@
         <v>60</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="D41" s="7"/>
     </row>
@@ -1203,7 +1203,7 @@
         <v>70</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C42" s="7"/>
     </row>
@@ -1212,10 +1212,10 @@
         <v>80</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="D43" s="7"/>
     </row>
@@ -1224,7 +1224,7 @@
         <v>90</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" s="7"/>
     </row>
@@ -1233,10 +1233,10 @@
         <v>100</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="17" t="s">
         <v>79</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1244,7 +1244,7 @@
         <v>200</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="7"/>
     </row>
@@ -1253,7 +1253,7 @@
         <v>400</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -1263,7 +1263,7 @@
         <v>800</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="7"/>
     </row>
@@ -1272,7 +1272,7 @@
         <v>1000</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49" s="7"/>
     </row>
@@ -1281,7 +1281,7 @@
         <v>2000</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" s="7"/>
     </row>
@@ -1317,7 +1317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1348,7 +1348,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1372,7 +1372,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1380,7 +1380,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1388,7 +1388,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.55000000000000004">
@@ -1396,7 +1396,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
@@ -1416,7 +1416,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1432,7 +1432,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1440,7 +1440,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>